<commit_message>
Kateryna - commit 13
</commit_message>
<xml_diff>
--- a/TestDataforSignUpFeature.xlsx
+++ b/TestDataforSignUpFeature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khait\IdeaProjects\bdd-sprint3-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F050151A-3CEB-48D4-9E7D-23AD585869D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524F9697-7FA7-4864-812F-BC69FEE8F4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8231E31C-7F69-4183-948E-CB53CED8EBA9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="129">
   <si>
     <t>First_name</t>
   </si>
@@ -411,13 +411,13 @@
     <t>test</t>
   </si>
   <si>
-    <t>cmcmeekan155@netvibes.com</t>
-  </si>
-  <si>
-    <t>cbreckenridge000@google.com</t>
-  </si>
-  <si>
     <t>SKIPPED</t>
+  </si>
+  <si>
+    <t>cmcmeekan02@netvibes.com</t>
+  </si>
+  <si>
+    <t>cbreckenridge22@google.com</t>
   </si>
   <si>
     <t>PASSED</t>
@@ -803,7 +803,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,7 +837,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -845,17 +847,19 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
@@ -863,13 +867,13 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -887,7 +891,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -905,7 +909,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -923,13 +927,11 @@
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
@@ -943,13 +945,11 @@
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -963,13 +963,11 @@
         <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
@@ -983,13 +981,11 @@
         <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1003,13 +999,11 @@
         <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1023,7 +1017,7 @@
         <v>42</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1041,7 +1035,7 @@
         <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1059,7 +1053,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1077,7 +1071,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1095,7 +1089,7 @@
         <v>58</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1113,7 +1107,7 @@
         <v>62</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1131,7 +1125,7 @@
         <v>66</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1149,7 +1143,7 @@
         <v>70</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1167,7 +1161,7 @@
         <v>74</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1185,7 +1179,7 @@
         <v>78</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1203,7 +1197,7 @@
         <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1221,7 +1215,7 @@
         <v>86</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1239,7 +1233,7 @@
         <v>90</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1257,7 +1251,7 @@
         <v>94</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1275,7 +1269,7 @@
         <v>98</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1293,7 +1287,7 @@
         <v>102</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1311,7 +1305,7 @@
         <v>106</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1329,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1347,7 +1341,7 @@
         <v>114</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1365,7 +1359,7 @@
         <v>118</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1383,7 +1377,7 @@
         <v>122</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1393,7 +1387,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1403,7 +1397,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>